<commit_message>
feat: se concluyo flujo 3 y flujo 4 queda pendiente casos de prueba adicionales
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/FlujosMCSS.xlsx
+++ b/src/main/resources/excel/FlujosMCSS.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="42">
   <si>
     <t>TC1</t>
   </si>
@@ -158,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +195,22 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -381,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -438,7 +454,11 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="42" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="43" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="44" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="45" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="46" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="47" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="48" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>

</xml_diff>